<commit_message>
Implementação de dos outros 2 casos de testes
</commit_message>
<xml_diff>
--- a/target/test-classes/br/com/rsinset/HUB_TDD/TestData/TestData.xlsx
+++ b/target/test-classes/br/com/rsinset/HUB_TDD/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willian.costa\eclipse-workspace\servlets\HUB_TDD\src\test\java\br\com\rsinset\HUB_TDD\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FBE7F5-3284-4D96-B1FA-636C1C608F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755192F0-BB1B-4469-8758-A4E583550DC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{9A238A30-1AA3-4A42-BD5B-6DAF71D155B8}"/>
   </bookViews>
@@ -129,7 +129,7 @@
     <t>5599-055</t>
   </si>
   <si>
-    <t>joao124</t>
+    <t>joao126</t>
   </si>
 </sst>
 </file>

</xml_diff>